<commit_message>
Initializing the SIQ document Updating tasks on PP "1st update" Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP.xlsx
+++ b/Software Deliveries Log/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65522B32-63B5-4346-8B1A-40A4D0E1819A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D4828F-9D02-4D8C-B313-19CE6D96A203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
   <si>
     <t>#</t>
   </si>
@@ -107,6 +107,42 @@
   </si>
   <si>
     <t>RTM_v1.0</t>
+  </si>
+  <si>
+    <t>Nouran Mamdouh</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Faliure</t>
+  </si>
+  <si>
+    <t>Donia Mohamed</t>
+  </si>
+  <si>
+    <t>Ahmed Refaat</t>
+  </si>
+  <si>
+    <t>Islam El-Bahnasawy</t>
+  </si>
+  <si>
+    <t>Marcelle Samir</t>
+  </si>
+  <si>
+    <t>CYRS-Document</t>
+  </si>
+  <si>
+    <t>Non-Technical</t>
+  </si>
+  <si>
+    <t>SRS-Document</t>
+  </si>
+  <si>
+    <t>HSI-Document</t>
+  </si>
+  <si>
+    <t>22-1-2020</t>
   </si>
 </sst>
 </file>
@@ -169,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,8 +272,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5B5B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -330,11 +378,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -357,9 +414,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -378,13 +432,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -393,19 +441,40 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -414,6 +483,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5B5B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -724,16 +798,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
   <dimension ref="A1:AO15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -750,158 +824,158 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="I2" s="15">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="I2" s="22">
         <v>43831</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15">
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22">
         <v>43862</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="22"/>
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22"/>
+      <c r="AO2" s="22"/>
     </row>
     <row r="3" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="I3" s="9">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="I3" s="8">
         <v>21</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="9">
         <v>22</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="9">
         <v>23</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="9">
         <v>24</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="9">
         <v>25</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="9">
         <v>26</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="9">
         <v>27</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="9">
         <v>28</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="Q3" s="9">
         <v>29</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="9">
         <v>30</v>
       </c>
-      <c r="S3" s="10">
+      <c r="S3" s="9">
         <v>31</v>
       </c>
-      <c r="T3" s="10">
+      <c r="T3" s="9">
         <v>1</v>
       </c>
-      <c r="U3" s="10">
+      <c r="U3" s="9">
         <v>2</v>
       </c>
-      <c r="V3" s="10">
+      <c r="V3" s="9">
         <v>3</v>
       </c>
-      <c r="W3" s="10">
+      <c r="W3" s="9">
         <v>4</v>
       </c>
-      <c r="X3" s="10">
+      <c r="X3" s="9">
         <v>5</v>
       </c>
-      <c r="Y3" s="10">
+      <c r="Y3" s="9">
         <v>6</v>
       </c>
-      <c r="Z3" s="10">
+      <c r="Z3" s="9">
         <v>7</v>
       </c>
-      <c r="AA3" s="10">
+      <c r="AA3" s="9">
         <v>8</v>
       </c>
-      <c r="AB3" s="10">
+      <c r="AB3" s="9">
         <v>9</v>
       </c>
-      <c r="AC3" s="10">
+      <c r="AC3" s="9">
         <v>10</v>
       </c>
-      <c r="AD3" s="10">
+      <c r="AD3" s="9">
         <v>11</v>
       </c>
-      <c r="AE3" s="10">
+      <c r="AE3" s="9">
         <v>12</v>
       </c>
-      <c r="AF3" s="10">
+      <c r="AF3" s="9">
         <v>13</v>
       </c>
-      <c r="AG3" s="10">
+      <c r="AG3" s="9">
         <v>14</v>
       </c>
-      <c r="AH3" s="10">
+      <c r="AH3" s="9">
         <v>15</v>
       </c>
-      <c r="AI3" s="10">
+      <c r="AI3" s="9">
         <v>16</v>
       </c>
-      <c r="AJ3" s="10">
+      <c r="AJ3" s="9">
         <v>17</v>
       </c>
-      <c r="AK3" s="10">
+      <c r="AK3" s="9">
         <v>18</v>
       </c>
-      <c r="AL3" s="10">
+      <c r="AL3" s="9">
         <v>19</v>
       </c>
-      <c r="AM3" s="10">
+      <c r="AM3" s="9">
         <v>20</v>
       </c>
-      <c r="AN3" s="10">
+      <c r="AN3" s="9">
         <v>21</v>
       </c>
-      <c r="AO3" s="11">
+      <c r="AO3" s="10">
         <v>22</v>
       </c>
     </row>
@@ -930,335 +1004,383 @@
       <c r="H4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="13" t="s">
+      <c r="N4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="P4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="S4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="13" t="s">
+      <c r="T4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="13" t="s">
+      <c r="U4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="V4" s="13" t="s">
+      <c r="V4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="W4" s="13" t="s">
+      <c r="W4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="13" t="s">
+      <c r="X4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Y4" s="13" t="s">
+      <c r="Y4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="Z4" s="13" t="s">
+      <c r="Z4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AA4" s="13" t="s">
+      <c r="AA4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="13" t="s">
+      <c r="AB4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AC4" s="13" t="s">
+      <c r="AC4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="13" t="s">
+      <c r="AD4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AE4" s="13" t="s">
+      <c r="AE4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="AF4" s="13" t="s">
+      <c r="AF4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AG4" s="13" t="s">
+      <c r="AG4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AH4" s="13" t="s">
+      <c r="AH4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AI4" s="13" t="s">
+      <c r="AI4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AJ4" s="13" t="s">
+      <c r="AJ4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AK4" s="13" t="s">
+      <c r="AK4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AL4" s="13" t="s">
+      <c r="AL4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="AM4" s="13" t="s">
+      <c r="AM4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="13" t="s">
+      <c r="AN4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AO4" s="14" t="s">
+      <c r="AO4" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="B5" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="16"/>
-      <c r="AD5" s="16"/>
-      <c r="AE5" s="16"/>
-      <c r="AF5" s="16"/>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="16"/>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="16"/>
-      <c r="AL5" s="16"/>
-      <c r="AM5" s="16"/>
-      <c r="AN5" s="16"/>
-      <c r="AO5" s="16"/>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="14"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="14"/>
+      <c r="AL5" s="14"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="14"/>
+      <c r="AO5" s="14"/>
+    </row>
+    <row r="6" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="B6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="16"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="16"/>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="16"/>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="16"/>
-      <c r="AL6" s="16"/>
-      <c r="AM6" s="16"/>
-      <c r="AN6" s="16"/>
-      <c r="AO6" s="16"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="14"/>
+      <c r="AH6" s="14"/>
+      <c r="AI6" s="14"/>
+      <c r="AJ6" s="14"/>
+      <c r="AK6" s="14"/>
+      <c r="AL6" s="14"/>
+      <c r="AM6" s="14"/>
+      <c r="AN6" s="14"/>
+      <c r="AO6" s="14"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="16"/>
-      <c r="AB7" s="16"/>
-      <c r="AC7" s="16"/>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="16"/>
-      <c r="AF7" s="16"/>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="16"/>
-      <c r="AI7" s="16"/>
-      <c r="AJ7" s="16"/>
-      <c r="AK7" s="16"/>
-      <c r="AL7" s="16"/>
-      <c r="AM7" s="16"/>
-      <c r="AN7" s="16"/>
-      <c r="AO7" s="16"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="14"/>
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="14"/>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="14"/>
+      <c r="AJ7" s="14"/>
+      <c r="AK7" s="14"/>
+      <c r="AL7" s="14"/>
+      <c r="AM7" s="14"/>
+      <c r="AN7" s="14"/>
+      <c r="AO7" s="14"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="16"/>
-      <c r="AD8" s="16"/>
-      <c r="AE8" s="16"/>
-      <c r="AF8" s="16"/>
-      <c r="AG8" s="16"/>
-      <c r="AH8" s="16"/>
-      <c r="AI8" s="16"/>
-      <c r="AJ8" s="16"/>
-      <c r="AK8" s="16"/>
-      <c r="AL8" s="16"/>
-      <c r="AM8" s="16"/>
-      <c r="AN8" s="16"/>
-      <c r="AO8" s="16"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="14"/>
+      <c r="AH8" s="14"/>
+      <c r="AI8" s="14"/>
+      <c r="AJ8" s="14"/>
+      <c r="AK8" s="14"/>
+      <c r="AL8" s="14"/>
+      <c r="AM8" s="14"/>
+      <c r="AN8" s="14"/>
+      <c r="AO8" s="14"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="16"/>
-      <c r="AI9" s="16"/>
-      <c r="AJ9" s="16"/>
-      <c r="AK9" s="16"/>
-      <c r="AL9" s="16"/>
-      <c r="AM9" s="16"/>
-      <c r="AN9" s="16"/>
-      <c r="AO9" s="16"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+      <c r="AH9" s="14"/>
+      <c r="AI9" s="14"/>
+      <c r="AJ9" s="14"/>
+      <c r="AK9" s="14"/>
+      <c r="AL9" s="14"/>
+      <c r="AM9" s="14"/>
+      <c r="AN9" s="14"/>
+      <c r="AO9" s="14"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>6</v>
-      </c>
+      <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1266,44 +1388,42 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="16"/>
-      <c r="AC10" s="16"/>
-      <c r="AD10" s="16"/>
-      <c r="AE10" s="16"/>
-      <c r="AF10" s="16"/>
-      <c r="AG10" s="16"/>
-      <c r="AH10" s="16"/>
-      <c r="AI10" s="16"/>
-      <c r="AJ10" s="16"/>
-      <c r="AK10" s="16"/>
-      <c r="AL10" s="16"/>
-      <c r="AM10" s="16"/>
-      <c r="AN10" s="16"/>
-      <c r="AO10" s="16"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="14"/>
+      <c r="AB10" s="14"/>
+      <c r="AC10" s="14"/>
+      <c r="AD10" s="14"/>
+      <c r="AE10" s="14"/>
+      <c r="AF10" s="14"/>
+      <c r="AG10" s="14"/>
+      <c r="AH10" s="14"/>
+      <c r="AI10" s="14"/>
+      <c r="AJ10" s="14"/>
+      <c r="AK10" s="14"/>
+      <c r="AL10" s="14"/>
+      <c r="AM10" s="14"/>
+      <c r="AN10" s="14"/>
+      <c r="AO10" s="14"/>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>7</v>
-      </c>
+      <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1311,44 +1431,42 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="16"/>
-      <c r="AC11" s="16"/>
-      <c r="AD11" s="16"/>
-      <c r="AE11" s="16"/>
-      <c r="AF11" s="16"/>
-      <c r="AG11" s="16"/>
-      <c r="AH11" s="16"/>
-      <c r="AI11" s="16"/>
-      <c r="AJ11" s="16"/>
-      <c r="AK11" s="16"/>
-      <c r="AL11" s="16"/>
-      <c r="AM11" s="16"/>
-      <c r="AN11" s="16"/>
-      <c r="AO11" s="16"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="14"/>
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="14"/>
+      <c r="AG11" s="14"/>
+      <c r="AH11" s="14"/>
+      <c r="AI11" s="14"/>
+      <c r="AJ11" s="14"/>
+      <c r="AK11" s="14"/>
+      <c r="AL11" s="14"/>
+      <c r="AM11" s="14"/>
+      <c r="AN11" s="14"/>
+      <c r="AO11" s="14"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>8</v>
-      </c>
+      <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1356,55 +1474,98 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
-      <c r="AA12" s="16"/>
-      <c r="AB12" s="16"/>
-      <c r="AC12" s="16"/>
-      <c r="AD12" s="16"/>
-      <c r="AE12" s="16"/>
-      <c r="AF12" s="16"/>
-      <c r="AG12" s="16"/>
-      <c r="AH12" s="16"/>
-      <c r="AI12" s="16"/>
-      <c r="AJ12" s="16"/>
-      <c r="AK12" s="16"/>
-      <c r="AL12" s="16"/>
-      <c r="AM12" s="16"/>
-      <c r="AN12" s="16"/>
-      <c r="AO12" s="16"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="14"/>
+      <c r="AE12" s="14"/>
+      <c r="AF12" s="14"/>
+      <c r="AG12" s="14"/>
+      <c r="AH12" s="14"/>
+      <c r="AI12" s="14"/>
+      <c r="AJ12" s="14"/>
+      <c r="AK12" s="14"/>
+      <c r="AL12" s="14"/>
+      <c r="AM12" s="14"/>
+      <c r="AN12" s="14"/>
+      <c r="AO12" s="14"/>
     </row>
     <row r="13" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I14" s="24"/>
-    </row>
-    <row r="15" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I15" s="23"/>
+    <row r="14" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="20"/>
+      <c r="J14" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+    </row>
+    <row r="15" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="19"/>
+      <c r="J15" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="D1:F3"/>
     <mergeCell ref="I2:S2"/>
     <mergeCell ref="T2:AO2"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
   </mergeCells>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{020FFF4C-682B-4AF7-A6AE-9B11809D486D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{020FFF4C-682B-4AF7-A6AE-9B11809D486D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I5</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1427,48 +1588,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1488,7 +1649,7 @@
       <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">

</xml_diff>

<commit_message>
Updated the PP after finishing the CYRS_V1.0 Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP.xlsx
+++ b/Software Deliveries Log/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D4828F-9D02-4D8C-B313-19CE6D96A203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6774D6B-3402-4AC2-BE68-EA6F5E061F05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -115,9 +115,6 @@
     <t>Progress</t>
   </si>
   <si>
-    <t>Faliure</t>
-  </si>
-  <si>
     <t>Donia Mohamed</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>22-1-2020</t>
+  </si>
+  <si>
+    <t>Overtime</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,6 +281,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF5B5B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -453,28 +459,34 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -799,7 +811,7 @@
   <dimension ref="A1:AO15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,61 +836,61 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="I2" s="22">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="I2" s="23">
         <v>43831</v>
       </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22">
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23">
         <v>43862</v>
       </c>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="22"/>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22"/>
-      <c r="AO2" s="22"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+      <c r="AG2" s="23"/>
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="23"/>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
     </row>
     <row r="3" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
       <c r="I3" s="8">
         <v>21</v>
       </c>
@@ -1108,25 +1120,25 @@
       <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="J5" s="30"/>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
@@ -1163,14 +1175,14 @@
       <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>28</v>
+      <c r="B6" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>20</v>
@@ -1180,8 +1192,8 @@
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="29"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
@@ -1219,24 +1231,24 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="J7" s="30"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
@@ -1274,24 +1286,24 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="J8" s="30"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
@@ -1329,24 +1341,24 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="F9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="30"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
@@ -1520,7 +1532,7 @@
     <row r="15" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="19"/>
       <c r="J15" s="26" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
@@ -1590,26 +1602,26 @@
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="23"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>

</xml_diff>

<commit_message>
Updating the PP according to new deliveries Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP.xlsx
+++ b/Software Deliveries Log/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2D5353-352C-4839-89F6-8A51756D6498}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829C72C4-FCAF-43BA-95F4-F12C4CE911F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
@@ -142,9 +142,6 @@
     <t>22-1-2020</t>
   </si>
   <si>
-    <t>Overtime</t>
-  </si>
-  <si>
     <t>23-1-2020</t>
   </si>
   <si>
@@ -152,13 +149,52 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>SRS-Modifications</t>
+  </si>
+  <si>
+    <t>CYRS-Modifications</t>
+  </si>
+  <si>
+    <t>HSI-Modifications</t>
+  </si>
+  <si>
+    <t>25-1-2020</t>
+  </si>
+  <si>
+    <t>26-1-2020</t>
+  </si>
+  <si>
+    <t>30-1-2020</t>
+  </si>
+  <si>
+    <t>29-1-2020</t>
+  </si>
+  <si>
+    <t>28-1-2020</t>
+  </si>
+  <si>
+    <t>Early Delivery</t>
+  </si>
+  <si>
+    <t>Late Delivery</t>
+  </si>
+  <si>
+    <t>CYRS_v1.1</t>
+  </si>
+  <si>
+    <t>SRS_v1.1</t>
+  </si>
+  <si>
+    <t>HIS_v1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,8 +249,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,12 +326,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF5B5B"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -296,6 +333,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -471,31 +526,52 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -531,7 +607,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1020535</xdr:colOff>
+      <xdr:colOff>935490</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>182336</xdr:rowOff>
     </xdr:to>
@@ -933,17 +1009,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
-  <dimension ref="A1:AO15"/>
+  <dimension ref="A1:AO17"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1261,10 +1337,10 @@
         <v>35</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="23"/>
@@ -1323,7 +1399,7 @@
         <v>35</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" s="23"/>
       <c r="J6" s="22"/>
@@ -1359,11 +1435,11 @@
       <c r="AN6" s="14"/>
       <c r="AO6" s="14"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1379,10 +1455,10 @@
         <v>35</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="23"/>
@@ -1418,11 +1494,11 @@
       <c r="AN7" s="14"/>
       <c r="AO7" s="14"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1438,10 +1514,10 @@
         <v>35</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="23"/>
@@ -1477,11 +1553,11 @@
       <c r="AN8" s="14"/>
       <c r="AO8" s="14"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1497,10 +1573,10 @@
         <v>35</v>
       </c>
       <c r="G9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="23"/>
@@ -1536,20 +1612,36 @@
       <c r="AN9" s="14"/>
       <c r="AO9" s="14"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+    <row r="10" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>6</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="30"/>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
@@ -1579,25 +1671,39 @@
       <c r="AN10" s="14"/>
       <c r="AO10" s="14"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+    <row r="11" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>7</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
       <c r="U11" s="14"/>
@@ -1622,25 +1728,39 @@
       <c r="AN11" s="14"/>
       <c r="AO11" s="14"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+    <row r="12" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>8</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
       <c r="S12" s="14"/>
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
@@ -1665,30 +1785,163 @@
       <c r="AN12" s="14"/>
       <c r="AO12" s="14"/>
     </row>
-    <row r="13" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>9</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="14"/>
+      <c r="AG13" s="14"/>
+      <c r="AH13" s="14"/>
+      <c r="AI13" s="14"/>
+      <c r="AJ13" s="14"/>
+      <c r="AK13" s="14"/>
+      <c r="AL13" s="14"/>
+      <c r="AM13" s="14"/>
+      <c r="AN13" s="14"/>
+      <c r="AO13" s="14"/>
+    </row>
     <row r="14" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I14" s="20"/>
-      <c r="J14" s="26" t="s">
+      <c r="A14" s="6">
+        <v>10</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
+      <c r="AG14" s="14"/>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="14"/>
+      <c r="AJ14" s="14"/>
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="14"/>
+      <c r="AM14" s="14"/>
+      <c r="AN14" s="14"/>
+      <c r="AO14" s="14"/>
+    </row>
+    <row r="15" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27"/>
+      <c r="B15" s="28"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-    </row>
-    <row r="15" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I15" s="19"/>
-      <c r="J15" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+    </row>
+    <row r="16" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+    </row>
+    <row r="17" spans="9:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I17" s="31"/>
+      <c r="J17" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
     <mergeCell ref="D1:F3"/>
     <mergeCell ref="I2:S2"/>
     <mergeCell ref="T2:AO2"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
   </mergeCells>
   <conditionalFormatting sqref="I5">
     <cfRule type="dataBar" priority="1">
@@ -1732,7 +1985,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,26 +2001,26 @@
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
@@ -1828,7 +2081,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1848,7 +2101,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1868,38 +2121,66 @@
         <v>20</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="B9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="B10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="B11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">

</xml_diff>

<commit_message>
Modifing the PP according to the changes in the SRS Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Deliveries Log/PP.xlsx
+++ b/Software Deliveries Log/PP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Deliveries Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829C72C4-FCAF-43BA-95F4-F12C4CE911F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0F2CFF-91B1-4A58-9530-24A4D5431CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7365D73D-1171-4AD1-8157-E0587B4CCD43}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="53">
   <si>
     <t>#</t>
   </si>
@@ -188,13 +188,16 @@
   </si>
   <si>
     <t>HIS_v1.1</t>
+  </si>
+  <si>
+    <t>31-1-2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +255,13 @@
     <font>
       <sz val="11"/>
       <color theme="4" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -461,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -532,6 +542,39 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -541,37 +584,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1011,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AD6F81-3C5E-45CC-B6D1-EBA8B52FB45E}">
   <dimension ref="A1:AO17"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,61 +1050,61 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="I2" s="25">
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="I2" s="36">
         <v>43831</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25">
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36">
         <v>43862</v>
       </c>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="25"/>
-      <c r="AH2" s="25"/>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="36"/>
+      <c r="AL2" s="36"/>
+      <c r="AM2" s="36"/>
+      <c r="AN2" s="36"/>
+      <c r="AO2" s="36"/>
     </row>
     <row r="3" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
       <c r="I3" s="8">
         <v>21</v>
       </c>
@@ -1640,8 +1653,8 @@
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="30"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="27"/>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
@@ -1690,7 +1703,9 @@
       <c r="F11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="H11" s="7" t="s">
         <v>38</v>
       </c>
@@ -1702,9 +1717,9 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
       <c r="P11" s="23"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="14"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="38"/>
       <c r="T11" s="14"/>
       <c r="U11" s="14"/>
       <c r="V11" s="14"/>
@@ -1747,7 +1762,9 @@
       <c r="F12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="H12" s="7" t="s">
         <v>38</v>
       </c>
@@ -1759,9 +1776,9 @@
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="14"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="22"/>
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
@@ -1817,7 +1834,7 @@
       <c r="M13" s="14"/>
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
-      <c r="P13" s="30"/>
+      <c r="P13" s="27"/>
       <c r="Q13" s="14"/>
       <c r="R13" s="14"/>
       <c r="S13" s="14"/>
@@ -1876,7 +1893,7 @@
       <c r="M14" s="14"/>
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
-      <c r="P14" s="30"/>
+      <c r="P14" s="27"/>
       <c r="Q14" s="14"/>
       <c r="R14" s="14"/>
       <c r="S14" s="14"/>
@@ -1904,44 +1921,44 @@
       <c r="AO14" s="14"/>
     </row>
     <row r="15" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
       <c r="I15" s="20"/>
-      <c r="J15" s="36" t="s">
+      <c r="J15" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
     </row>
     <row r="16" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
       <c r="I16" s="19"/>
-      <c r="J16" s="34" t="s">
+      <c r="J16" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
     </row>
     <row r="17" spans="9:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I17" s="31"/>
-      <c r="J17" s="32" t="s">
+      <c r="I17" s="28"/>
+      <c r="J17" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T2:AO2"/>
     <mergeCell ref="J15:M15"/>
     <mergeCell ref="J16:M16"/>
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="D1:F3"/>
     <mergeCell ref="I2:S2"/>
-    <mergeCell ref="T2:AO2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5">
     <cfRule type="dataBar" priority="1">
@@ -1984,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84E9320-5BEB-4411-BFD0-20ED4C434367}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,26 +2018,26 @@
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="26"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
     </row>
@@ -2160,7 +2177,9 @@
       <c r="E10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">

</xml_diff>